<commit_message>
Fixed: better date time conversion (convert_to_datetime method) using real examples. Logic on iPad. NEXT TODO: Method is starting to get complicated: put into separate file? also work on helper for dealing with before/after
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EEEBE082-F47A-974F-A625-D3E1B751C5D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7225E79-CDED-3246-9C94-925AEB91FC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -132,9 +132,6 @@
     <t>Free after 17h30</t>
   </si>
   <si>
-    <t>Free after 15h, but not all the time</t>
-  </si>
-  <si>
     <t>Free after 17h</t>
   </si>
   <si>
@@ -223,6 +220,9 @@
   </si>
   <si>
     <t>I get my work schedule a week before so I might work Thursdays or Fridays. I can teach if you can't find a teacher.</t>
+  </si>
+  <si>
+    <t>Free after 15h</t>
   </si>
 </sst>
 </file>
@@ -610,11 +610,12 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="1" max="1" width="57.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
@@ -783,36 +784,36 @@
         <v>32</v>
       </c>
       <c r="E7" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="F7" s="3" t="s">
+      <c r="G7" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="G7" s="3" t="s">
+      <c r="H7" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="H7" s="3" t="s">
+      <c r="I7" s="4" t="s">
         <v>36</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" s="3" t="s">
         <v>38</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>39</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>31</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>28</v>
@@ -821,33 +822,33 @@
         <v>11</v>
       </c>
       <c r="H8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>41</v>
-      </c>
-      <c r="I8" s="3" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3" t="s">
+      <c r="D9" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D9" s="3" t="s">
+      <c r="E9" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="F9" s="3" t="s">
+      <c r="G9" s="3" t="s">
         <v>46</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>47</v>
       </c>
       <c r="H9" s="3" t="s">
         <v>11</v>
@@ -856,80 +857,80 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="C10" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="D10" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="D10" s="3" t="s">
+      <c r="E10" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="E10" s="3" t="s">
+      <c r="F10" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="G10" s="3" t="s">
         <v>52</v>
-      </c>
-      <c r="F10" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="G10" s="3" t="s">
-        <v>53</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C11" s="3" t="s">
+      <c r="D11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="G11" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="D11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="G11" s="3" t="s">
+      <c r="H11" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>57</v>
-      </c>
-      <c r="H11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D12" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="D12" s="3" t="s">
+      <c r="E12" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="F12" s="3" t="s">
         <v>61</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>62</v>
       </c>
       <c r="G12" s="3" t="s">
         <v>18</v>
@@ -938,7 +939,7 @@
         <v>18</v>
       </c>
       <c r="I12" s="3" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
bef_betw_aft method after/before good, need to do between. Also need to check logic (on ipad) for what to do in the no Free case.
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7225E79-CDED-3246-9C94-925AEB91FC10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A28B2F-3100-2B4F-9E53-68696048E3DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
@@ -610,7 +610,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="H6" sqref="H6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
tested out with first 4 members from twice team (yas) - next, add oceanne and implement between in bef_betw_aft() method
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10917"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2A28B2F-3100-2B4F-9E53-68696048E3DE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074036BD-A954-F245-A014-728AB764B2A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -223,6 +223,12 @@
   </si>
   <si>
     <t>Free after 15h</t>
+  </si>
+  <si>
+    <t>Free after 5:30pm</t>
+  </si>
+  <si>
+    <t>before 9:30pm</t>
   </si>
 </sst>
 </file>
@@ -610,7 +616,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -666,7 +672,7 @@
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>13</v>
+        <v>64</v>
       </c>
       <c r="D3" s="3" t="s">
         <v>14</v>
@@ -681,7 +687,7 @@
         <v>15</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>11</v>
+        <v>65</v>
       </c>
       <c r="I3" s="3" t="s">
         <v>16</v>

</xml_diff>

<commit_message>
fixed bug that came up during testing with superm team (:30) gave wrong schedule
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{074036BD-A954-F245-A014-728AB764B2A4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E55560-A8CB-A045-9CB8-49E41B751F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="560" windowWidth="28040" windowHeight="17440" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="300" yWindow="1920" windowWidth="31720" windowHeight="18540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="87">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -229,6 +230,69 @@
   </si>
   <si>
     <t>before 9:30pm</t>
+  </si>
+  <si>
+    <t>Sam</t>
+  </si>
+  <si>
+    <t>After 5</t>
+  </si>
+  <si>
+    <t>Kevin</t>
+  </si>
+  <si>
+    <t>Free after 5 pm</t>
+  </si>
+  <si>
+    <t>Yutong</t>
+  </si>
+  <si>
+    <t>Em Y.</t>
+  </si>
+  <si>
+    <t>After 6pm</t>
+  </si>
+  <si>
+    <t>Cindy</t>
+  </si>
+  <si>
+    <t>After 6</t>
+  </si>
+  <si>
+    <t>After 12h</t>
+  </si>
+  <si>
+    <t>After 6h</t>
+  </si>
+  <si>
+    <t>After 10 am</t>
+  </si>
+  <si>
+    <t>Free except 16h45-18h15</t>
+  </si>
+  <si>
+    <t>Seasy</t>
+  </si>
+  <si>
+    <t>After 6:30</t>
+  </si>
+  <si>
+    <t>After 5:30</t>
+  </si>
+  <si>
+    <t>After 4</t>
+  </si>
+  <si>
+    <t>Christine</t>
+  </si>
+  <si>
+    <t>After 5pm</t>
+  </si>
+  <si>
+    <t>after 4pm</t>
+  </si>
+  <si>
+    <t>SUPERM (7) - JOPPING - DUE FRIDAY OCT 11 9:00PM</t>
   </si>
 </sst>
 </file>
@@ -612,11 +676,253 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74780E18-0271-3344-9AE4-771AE2C0452F}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:A9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>85</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=pAnK1y7qjuE" xr:uid="{93F4B0EA-5557-8B43-94E1-699F521485A5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89D4D5-A1AB-C148-BF69-36469C4FA223}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
1) deleted oldconverttodt() from dtconvert, 2) dealing with except - realized that DT CONVERSION has to be moved INSIDE bef_betw_aft() (before: was in convert_to_dt()), 3) added (messy) helper methods: extract_again() and french() - to help with between/except, 4) a Lot of debugging. NEXT: implement between in bef_betw_aft(), delete comments in convert_to_datetime()
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3E55560-A8CB-A045-9CB8-49E41B751F40}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE275636-2854-E044-82C6-8D05D9C0F2C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="300" yWindow="1920" windowWidth="31720" windowHeight="18540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="88">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -293,6 +293,9 @@
   </si>
   <si>
     <t>SUPERM (7) - JOPPING - DUE FRIDAY OCT 11 9:00PM</t>
+  </si>
+  <si>
+    <t>Free except 16h30-18h30</t>
   </si>
 </sst>
 </file>
@@ -680,7 +683,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:A9"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -851,7 +854,7 @@
         <v>11</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="J7" s="3" t="s">
         <v>78</v>

</xml_diff>

<commit_message>
deleted comments in convert_to_datetime(), implemented BETWEEN in bef_betw_aft()
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE275636-2854-E044-82C6-8D05D9C0F2C3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C597831F-E617-564F-9958-BE62D3CB43CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="2320" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="88">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="89">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -268,9 +268,6 @@
     <t>After 10 am</t>
   </si>
   <si>
-    <t>Free except 16h45-18h15</t>
-  </si>
-  <si>
     <t>Seasy</t>
   </si>
   <si>
@@ -296,6 +293,12 @@
   </si>
   <si>
     <t>Free except 16h30-18h30</t>
+  </si>
+  <si>
+    <t>Free between 16h45-18h15</t>
+  </si>
+  <si>
+    <t>not avai</t>
   </si>
 </sst>
 </file>
@@ -683,7 +686,7 @@
   <dimension ref="A1:J9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -695,7 +698,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -750,7 +753,7 @@
         <v>67</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>10</v>
+        <v>88</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
@@ -854,15 +857,15 @@
         <v>11</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="3" t="s">
         <v>87</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -871,16 +874,16 @@
         <v>67</v>
       </c>
       <c r="D8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="3" t="s">
         <v>80</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>81</v>
       </c>
       <c r="F8" s="3" t="s">
         <v>67</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>11</v>
@@ -888,7 +891,7 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
@@ -897,19 +900,19 @@
         <v>50</v>
       </c>
       <c r="D9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>84</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>85</v>
       </c>
     </row>
   </sheetData>
@@ -925,7 +928,7 @@
   <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+      <selection activeCell="D28" sqref="D28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
started fixing weird error with hr
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C597831F-E617-564F-9958-BE62D3CB43CE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E0191A-74E4-EE4B-814D-1ED52B6400B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -682,253 +682,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74780E18-0271-3344-9AE4-771AE2C0452F}">
-  <dimension ref="A1:J9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>68</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>70</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>71</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>72</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>74</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>75</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>76</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>79</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>80</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>81</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
-      <c r="A9" s="3" t="s">
-        <v>82</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>84</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=pAnK1y7qjuE" xr:uid="{93F4B0EA-5557-8B43-94E1-699F521485A5}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89D4D5-A1AB-C148-BF69-36469C4FA223}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D28" sqref="D28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -977,288 +735,288 @@
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
+      <c r="A3" s="4" t="s">
+        <v>30</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>64</v>
+        <v>31</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>14</v>
+        <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>11</v>
+        <v>63</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>14</v>
+        <v>33</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>16</v>
+        <v>35</v>
+      </c>
+      <c r="I3" s="4" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>17</v>
+        <v>37</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>18</v>
+        <v>38</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="D4" s="3" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>20</v>
+        <v>28</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I4" s="3"/>
+        <v>40</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>13</v>
+        <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>23</v>
+        <v>43</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>22</v>
+        <v>45</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>11</v>
+        <v>46</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="I5" s="3" t="s">
-        <v>24</v>
-      </c>
+      <c r="I5" s="3"/>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>25</v>
+        <v>47</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>26</v>
+        <v>48</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>10</v>
+        <v>49</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>28</v>
+        <v>51</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>11</v>
+        <v>50</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I6" s="3"/>
+        <v>18</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>30</v>
+      <c r="A7" s="3" t="s">
+        <v>54</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>31</v>
+        <v>55</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>32</v>
+        <v>55</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>34</v>
+        <v>56</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I7" s="4" t="s">
-        <v>36</v>
+        <v>11</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>57</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>37</v>
+      <c r="A8" s="2" t="s">
+        <v>58</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>39</v>
+        <v>60</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>39</v>
+        <v>59</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>40</v>
+        <v>18</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>41</v>
+        <v>62</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>43</v>
+        <v>64</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>44</v>
+        <v>14</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>43</v>
+        <v>11</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>45</v>
+        <v>14</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>46</v>
+        <v>15</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I9" s="3"/>
+        <v>65</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>49</v>
+        <v>19</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>51</v>
+        <v>20</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>50</v>
+        <v>20</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>52</v>
+        <v>20</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="I10" s="3" t="s">
-        <v>53</v>
-      </c>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>54</v>
+        <v>21</v>
       </c>
       <c r="B11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>55</v>
+        <v>13</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>55</v>
+        <v>23</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>55</v>
+        <v>22</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>56</v>
+        <v>11</v>
       </c>
       <c r="H11" s="3" t="s">
         <v>11</v>
       </c>
       <c r="I11" s="3" t="s">
-        <v>57</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="2" t="s">
-        <v>58</v>
+      <c r="A12" s="3" t="s">
+        <v>25</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>18</v>
+        <v>26</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>59</v>
+        <v>10</v>
       </c>
       <c r="D12" s="3" t="s">
-        <v>60</v>
+        <v>27</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="F12" s="3" t="s">
-        <v>61</v>
+        <v>11</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="H12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I12" s="3" t="s">
-        <v>62</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="I12" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1266,4 +1024,246 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74780E18-0271-3344-9AE4-771AE2C0452F}">
+  <dimension ref="A1:J9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="13.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="21.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>84</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=pAnK1y7qjuE" xr:uid="{93F4B0EA-5557-8B43-94E1-699F521485A5}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
bug seems to be fixed, works for twice now
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5E0191A-74E4-EE4B-814D-1ED52B6400B9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B658CAA2-D51C-5C4C-BB1B-FFE7B624F1FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -166,15 +166,9 @@
     <t>Free after 4:30</t>
   </si>
   <si>
-    <t>Free before 4/after 5:30</t>
-  </si>
-  <si>
     <t>Free after 5:30</t>
   </si>
   <si>
-    <t>Free before 3:30/after 4:30</t>
-  </si>
-  <si>
     <t>laura</t>
   </si>
   <si>
@@ -196,18 +190,6 @@
     <t>i get my work schedule a week ahead. sept 27, cant between 9 and 12 and 29 before 6pm</t>
   </si>
   <si>
-    <t>Brandon</t>
-  </si>
-  <si>
-    <t>Libre après 18h</t>
-  </si>
-  <si>
-    <t>Libre après 17h</t>
-  </si>
-  <si>
-    <t>Pas disponible le 27 septembre</t>
-  </si>
-  <si>
     <t>Johanne</t>
   </si>
   <si>
@@ -299,6 +281,12 @@
   </si>
   <si>
     <t>not avai</t>
+  </si>
+  <si>
+    <t>Free except 4-5:30</t>
+  </si>
+  <si>
+    <t>Free except 3:30-4:30</t>
   </si>
 </sst>
 </file>
@@ -683,21 +671,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89D4D5-A1AB-C148-BF69-36469C4FA223}">
-  <dimension ref="A1:I12"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+      <selection activeCell="A7" sqref="A7:XFD7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="57.1640625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="28" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="13" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
@@ -748,7 +737,7 @@
         <v>32</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
       <c r="F3" s="3" t="s">
         <v>33</v>
@@ -803,16 +792,16 @@
         <v>43</v>
       </c>
       <c r="D5" s="3" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>43</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="G5" s="3" t="s">
-        <v>46</v>
+        <v>84</v>
       </c>
       <c r="H5" s="3" t="s">
         <v>11</v>
@@ -821,202 +810,173 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B6" s="3" t="s">
+      <c r="D6" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C6" s="3" t="s">
+      <c r="E6" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="3" t="s">
         <v>50</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>52</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>18</v>
       </c>
       <c r="I6" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C7" s="3" t="s">
         <v>53</v>
       </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
+      <c r="D7" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>55</v>
-      </c>
       <c r="E7" s="3" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F7" s="3" t="s">
         <v>55</v>
       </c>
       <c r="G7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>57</v>
-      </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C8" s="3" t="s">
+      <c r="D8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="3" t="s">
         <v>59</v>
       </c>
-      <c r="D8" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>18</v>
-      </c>
       <c r="I8" s="3" t="s">
-        <v>62</v>
+        <v>16</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>14</v>
+        <v>20</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="I9" s="3" t="s">
-        <v>16</v>
-      </c>
+        <v>18</v>
+      </c>
+      <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>20</v>
+        <v>11</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="I10" s="3"/>
+        <v>11</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="D11" s="3" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="E11" s="3" t="s">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F11" s="3" t="s">
-        <v>22</v>
+        <v>11</v>
       </c>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>29</v>
       </c>
       <c r="H11" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I11" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A12" s="3" t="s">
-        <v>25</v>
-      </c>
-      <c r="B12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C12" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G12" s="3" t="s">
-        <v>29</v>
-      </c>
-      <c r="H12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="I12" s="3"/>
+      <c r="I11" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -1043,7 +1003,7 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
@@ -1077,51 +1037,51 @@
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G3" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="H3" s="3" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>31</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>11</v>
@@ -1129,7 +1089,7 @@
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>22</v>
@@ -1150,15 +1110,15 @@
         <v>22</v>
       </c>
       <c r="H5" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>31</v>
@@ -1181,54 +1141,54 @@
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="H8" s="3" t="s">
         <v>11</v>
@@ -1236,28 +1196,28 @@
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
-        <v>82</v>
+        <v>76</v>
       </c>
       <c r="B9" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>84</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
next: fix cant x-xpm error'
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,13 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B658CAA2-D51C-5C4C-BB1B-FFE7B624F1FC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C340704-86D4-1644-928C-B973AEFA8C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2320" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="4" sheetId="4" r:id="rId1"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="118">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -287,13 +289,115 @@
   </si>
   <si>
     <t>Free except 3:30-4:30</t>
+  </si>
+  <si>
+    <t>Moose</t>
+  </si>
+  <si>
+    <t>Not Avaiable</t>
+  </si>
+  <si>
+    <t>Guada</t>
+  </si>
+  <si>
+    <t>Free after 6:30pm</t>
+  </si>
+  <si>
+    <t>Penn</t>
+  </si>
+  <si>
+    <t>after 4:00</t>
+  </si>
+  <si>
+    <t>free after 5:30</t>
+  </si>
+  <si>
+    <t>Zheng</t>
+  </si>
+  <si>
+    <t>Free after 3</t>
+  </si>
+  <si>
+    <t>Free after 6</t>
+  </si>
+  <si>
+    <t>Free after 7</t>
+  </si>
+  <si>
+    <t>Free after 4</t>
+  </si>
+  <si>
+    <t>Yuta</t>
+  </si>
+  <si>
+    <t>After 6h30</t>
+  </si>
+  <si>
+    <t>I am free on sundays and on Monday but this coming long weekend, I am not availble from Friday to Monday. Please note only this Sunday I am not available. I told you my achedule was rip 😆😅</t>
+  </si>
+  <si>
+    <t>cant on octo14 15 16 and 23</t>
+  </si>
+  <si>
+    <t>Seventeen practices (10th 12th [12-14] 15th [6-8]), 
+cant 18-20, 
+rain filming sunday 13th at 7, 
+Cant 25th and 26th</t>
+  </si>
+  <si>
+    <t>Can't before Oct 18. Plz plz plz not rushed I basically have midterms every week until finals.</t>
+  </si>
+  <si>
+    <t>moriann group 1</t>
+  </si>
+  <si>
+    <t>After 4pm</t>
+  </si>
+  <si>
+    <t>after 5</t>
+  </si>
+  <si>
+    <t>Jessica</t>
+  </si>
+  <si>
+    <t>Free after 2pm</t>
+  </si>
+  <si>
+    <t>Free until 3pm</t>
+  </si>
+  <si>
+    <t>Free after 6pm</t>
+  </si>
+  <si>
+    <t>Oceanne</t>
+  </si>
+  <si>
+    <t>Not free</t>
+  </si>
+  <si>
+    <t>Free between 12-16h</t>
+  </si>
+  <si>
+    <t>can't 1-5</t>
+  </si>
+  <si>
+    <t>can't after 6pm</t>
+  </si>
+  <si>
+    <t>can't before 1pm</t>
+  </si>
+  <si>
+    <t>moriann group 2</t>
+  </si>
+  <si>
+    <t>except 6-8</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -328,6 +432,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -350,12 +460,16 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -670,11 +784,450 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926DF328-B4D7-7A40-880B-B5026507095A}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I12" sqref="I12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="150" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=3ymwOvzhwHs" xr:uid="{AD516D4B-458B-B247-8E46-E05E6F943E49}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7F069-2B14-EB4E-B090-4721D7B9CDF9}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="150" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=3ymwOvzhwHs" xr:uid="{0B1E64AB-53FC-3449-BD43-F87EF605ACB3}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89D4D5-A1AB-C148-BF69-36469C4FA223}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7:XFD7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="A1:I2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -986,7 +1539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74780E18-0271-3344-9AE4-771AE2C0452F}">
   <dimension ref="A1:J9"/>
   <sheetViews>

</xml_diff>

<commit_message>
fixed cant x-xpm error: added _if cant_ statement in convert_to_datetime()
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C340704-86D4-1644-928C-B973AEFA8C07}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5F095B-317B-0944-8D90-0ACCE87FEF00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="1280" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
     <sheet name="4" sheetId="4" r:id="rId1"/>
@@ -788,7 +788,7 @@
   <dimension ref="A1:I9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I12" sqref="I12"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
nvm the grid right now: do datetime date method first (include dates in practice schedules, not just times) - in get_practice_range helper, use comb
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD5F095B-317B-0944-8D90-0ACCE87FEF00}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEFA26F-7EC4-C748-91C2-EF95063C39B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
-    <sheet name="4" sheetId="4" r:id="rId1"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="4" sheetId="4" r:id="rId2"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
@@ -784,450 +784,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926DF328-B4D7-7A40-880B-B5026507095A}">
-  <dimension ref="A1:I9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D15" sqref="D15"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="150" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>108</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>110</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>111</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>83</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="G8" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="H8" s="3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="D9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="E9" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="F9" s="3" t="s">
-        <v>113</v>
-      </c>
-      <c r="G9" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H9" s="3" t="s">
-        <v>115</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=3ymwOvzhwHs" xr:uid="{AD516D4B-458B-B247-8E46-E05E6F943E49}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7F069-2B14-EB4E-B090-4721D7B9CDF9}">
-  <dimension ref="A1:I7"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:XFD40"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="9" max="9" width="150" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A1" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="G2" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
-        <v>85</v>
-      </c>
-      <c r="B3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>86</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I3" s="3"/>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="D4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="E4" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="F4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="G4" s="3" t="s">
-        <v>88</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="I4" s="3" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="B5" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C5" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>91</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="G5" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>92</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="G6" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="6" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>97</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I7" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-  </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=3ymwOvzhwHs" xr:uid="{0B1E64AB-53FC-3449-BD43-F87EF605ACB3}"/>
-  </hyperlinks>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89D4D5-A1AB-C148-BF69-36469C4FA223}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="A1:I2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1534,6 +1095,445 @@
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=3ymwOvzhwHs" xr:uid="{154F0FCC-13BC-404F-96F4-A7D8AB41C904}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926DF328-B4D7-7A40-880B-B5026507095A}">
+  <dimension ref="A1:I9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D15" sqref="D15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="12.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="22.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="150" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>112</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>84</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>117</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H9" s="3" t="s">
+        <v>115</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=3ymwOvzhwHs" xr:uid="{AD516D4B-458B-B247-8E46-E05E6F943E49}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7F069-2B14-EB4E-B090-4721D7B9CDF9}">
+  <dimension ref="A1:I7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A8" sqref="A8:XFD40"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="9" max="9" width="150" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="C3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I3" s="3"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>89</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>90</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>91</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="57" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="6" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://www.youtube.com/watch?v=3ymwOvzhwHs" xr:uid="{0B1E64AB-53FC-3449-BD43-F87EF605ACB3}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
get_practice_range returns r_comb, a 2d list of datetime times. NEXT: use/fix get_dt_date method and r_comb to get SUGGESTED practice dates
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DEFA26F-7EC4-C748-91C2-EF95063C39B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191A1F03-EE9D-7C4B-A80F-F2065A4323C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="119">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -391,13 +391,16 @@
   </si>
   <si>
     <t>except 6-8</t>
+  </si>
+  <si>
+    <t>except 2-4pm</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -438,6 +441,13 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -460,7 +470,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -470,6 +480,7 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -788,7 +799,7 @@
   <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -973,8 +984,8 @@
       <c r="G7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="H7" s="3" t="s">
-        <v>18</v>
+      <c r="H7" s="7" t="s">
+        <v>118</v>
       </c>
       <c r="I7" s="3" t="s">
         <v>56</v>

</xml_diff>

<commit_message>
add n and sheet name as inputs from command line
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -1,22 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11013"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{191A1F03-EE9D-7C4B-A80F-F2065A4323C7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351B128F-BC2D-254F-BE60-A6A89FD8188D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="38160" yWindow="-700" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="4" sheetId="4" r:id="rId2"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId4"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
+    <sheet name="4" sheetId="4" r:id="rId3"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -34,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="119">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="142">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -394,6 +395,75 @@
   </si>
   <si>
     <t>except 2-4pm</t>
+  </si>
+  <si>
+    <t>[RUSHED] EXO - OBSESSION - DUE WED NOV 27 9:00PM</t>
+  </si>
+  <si>
+    <t>Not free from 2h30-6h</t>
+  </si>
+  <si>
+    <t>Free after 12h</t>
+  </si>
+  <si>
+    <t>After 12h30</t>
+  </si>
+  <si>
+    <t>Not free from 16h45-18h15</t>
+  </si>
+  <si>
+    <t>Nothing on DEC.4 PLZ (allow i think filming on dec 7/8 is doable) ALSO maybe 3-4 practices?</t>
+  </si>
+  <si>
+    <t>Joëlle</t>
+  </si>
+  <si>
+    <t>Before 6pm</t>
+  </si>
+  <si>
+    <t>** Workshift end at 5pm. Pls, this really devoted exo-l really want to do it :')</t>
+  </si>
+  <si>
+    <t>After 2</t>
+  </si>
+  <si>
+    <t>Sean</t>
+  </si>
+  <si>
+    <t>After 1</t>
+  </si>
+  <si>
+    <t>Can I be Kai? c: uwu</t>
+  </si>
+  <si>
+    <t>Juliana</t>
+  </si>
+  <si>
+    <t>After 3</t>
+  </si>
+  <si>
+    <t>Janet</t>
+  </si>
+  <si>
+    <t>Before 3</t>
+  </si>
+  <si>
+    <t>Before 5</t>
+  </si>
+  <si>
+    <t>Saturday it depends on my job</t>
+  </si>
+  <si>
+    <t>Justine</t>
+  </si>
+  <si>
+    <t>Free after 7pm</t>
+  </si>
+  <si>
+    <t>wanna be either kai or sehun :D //will filming be b4 the holidays? (im gone on the 24th of dec)</t>
+  </si>
+  <si>
+    <t>After 5:30pm</t>
   </si>
 </sst>
 </file>
@@ -795,10 +865,234 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AA26D7-45B2-1A4A-91B0-76F117F9AA59}">
+  <dimension ref="A1:I8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B12" sqref="B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="3"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>136</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>140</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://youtu.be/gb7U2QO6MZk" xr:uid="{E721F06D-027F-014B-A49D-DFBF8949B0F8}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89D4D5-A1AB-C148-BF69-36469C4FA223}">
   <dimension ref="A1:I11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
@@ -1111,7 +1405,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926DF328-B4D7-7A40-880B-B5026507095A}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -1352,7 +1646,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7F069-2B14-EB4E-B090-4721D7B9CDF9}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -1550,7 +1844,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74780E18-0271-3344-9AE4-771AE2C0452F}">
   <dimension ref="A1:J9"/>
   <sheetViews>

</xml_diff>

<commit_message>
added cmd line arguments: next, implement generate_practice_times_2
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{351B128F-BC2D-254F-BE60-A6A89FD8188D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97CE76DF-72B3-B648-A537-8E871D1660A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38160" yWindow="-700" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="338" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="356" uniqueCount="145">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -424,9 +424,15 @@
     <t>** Workshift end at 5pm. Pls, this really devoted exo-l really want to do it :')</t>
   </si>
   <si>
+    <t>Karen</t>
+  </si>
+  <si>
     <t>After 2</t>
   </si>
   <si>
+    <t>Finish in 2 practice ? :D</t>
+  </si>
+  <si>
     <t>Sean</t>
   </si>
   <si>
@@ -440,6 +446,9 @@
   </si>
   <si>
     <t>After 3</t>
+  </si>
+  <si>
+    <t>The only Sunday I wont be free is December 1st. Other than that my schedule is good.</t>
   </si>
   <si>
     <t>Janet</t>
@@ -470,7 +479,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -518,6 +527,28 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <strike/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -540,7 +571,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -551,6 +582,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -866,10 +900,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AA26D7-45B2-1A4A-91B0-76F117F9AA59}">
-  <dimension ref="A1:I8"/>
+  <dimension ref="A1:I10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -951,13 +985,13 @@
         <v>126</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>11</v>
@@ -966,47 +1000,47 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
+    <row r="5" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A5" s="8" t="s">
+        <v>128</v>
+      </c>
+      <c r="B5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="9" t="s">
         <v>129</v>
       </c>
-      <c r="B5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C5" s="3" t="s">
+      <c r="E5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="9" t="s">
+        <v>31</v>
+      </c>
+      <c r="H5" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="8" t="s">
         <v>130</v>
-      </c>
-      <c r="D5" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="E5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="F5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I5" s="3" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
         <v>132</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>68</v>
-      </c>
       <c r="D6" s="3" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>31</v>
@@ -1015,69 +1049,127 @@
         <v>31</v>
       </c>
       <c r="G6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="H6" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I6" s="3"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>134</v>
       </c>
       <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G7" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="C7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>130</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>128</v>
-      </c>
       <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="3"/>
+    </row>
+    <row r="8" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="8" t="s">
+        <v>87</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="E8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="8" t="s">
+        <v>58</v>
+      </c>
+      <c r="H8" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="I8" s="8" t="s">
         <v>136</v>
       </c>
-      <c r="I7" s="3" t="s">
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="3" t="s">
         <v>137</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
+      <c r="B9" s="3" t="s">
         <v>138</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="G8" s="3" t="s">
+      <c r="C9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F9" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="H9" s="3" t="s">
         <v>139</v>
       </c>
-      <c r="H8" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="I8" s="3" t="s">
+      <c r="I9" s="3" t="s">
         <v>140</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A10" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>142</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>143</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
worked out the multiple member print, need to fix the dates of the week to align
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB2BAB2-B978-9D41-8C25-5B76DFA3A339}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907C6BF4-AEBC-704E-96DC-50CD21B43A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="20540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet4" sheetId="5" r:id="rId1"/>
-    <sheet name="Sheet1" sheetId="1" r:id="rId2"/>
-    <sheet name="4" sheetId="4" r:id="rId3"/>
-    <sheet name="Sheet3" sheetId="3" r:id="rId4"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId5"/>
+    <sheet name="Sheet4 (2)" sheetId="6" r:id="rId1"/>
+    <sheet name="Sheet4" sheetId="5" r:id="rId2"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
+    <sheet name="4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet3" sheetId="3" r:id="rId5"/>
+    <sheet name="Sheet2" sheetId="2" r:id="rId6"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="135">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -845,11 +846,148 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96FCFC8-74A0-4B4A-A658-B299719390AA}">
+  <dimension ref="A1:I5"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="I3" s="3" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>126</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A5" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I5" s="3"/>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" display="https://youtu.be/gb7U2QO6MZk" xr:uid="{0F3C221A-1C81-4744-9572-CE1DEB193F95}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A6AA26D7-45B2-1A4A-91B0-76F117F9AA59}">
   <dimension ref="A1:I8"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1066,7 +1204,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FA89D4D5-A1AB-C148-BF69-36469C4FA223}">
   <dimension ref="A1:I11"/>
   <sheetViews>
@@ -1383,7 +1521,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926DF328-B4D7-7A40-880B-B5026507095A}">
   <dimension ref="A1:I9"/>
   <sheetViews>
@@ -1624,7 +1762,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1B7F069-2B14-EB4E-B090-4721D7B9CDF9}">
   <dimension ref="A1:I7"/>
   <sheetViews>
@@ -1822,7 +1960,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{74780E18-0271-3344-9AE4-771AE2C0452F}">
   <dimension ref="A1:J9"/>
   <sheetViews>

</xml_diff>

<commit_message>
finished visualize_ex_week(), next work on finishing implementation of generate_practice_times_2()
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{907C6BF4-AEBC-704E-96DC-50CD21B43A8D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B6E6D2-EA5F-FD44-879A-4C15872E4F38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="135">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -847,20 +847,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C96FCFC8-74A0-4B4A-A658-B299719390AA}">
-  <dimension ref="A1:I5"/>
+  <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="A8" sqref="A8:H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -889,7 +889,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>67</v>
       </c>
@@ -918,7 +918,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>125</v>
       </c>
@@ -947,7 +947,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>129</v>
       </c>
@@ -973,6 +973,95 @@
         <v>11</v>
       </c>
       <c r="I5" s="3"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A6" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="M6" s="8"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A7" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="F7" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="G7" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I7" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A8" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I8" s="3"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -987,7 +1076,7 @@
   <dimension ref="A1:I8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J16" sqref="J16"/>
+      <selection activeCell="A6" sqref="A6:M11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
NEXT TODO: see ipad
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7B6E6D2-EA5F-FD44-879A-4C15872E4F38}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2261A5-F73D-F749-8217-3A84FFEB9A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="399" uniqueCount="136">
   <si>
     <t>TWICE (9) - FEEL SPECIAL [SEMI-RUSH] - DUE THURS SEP 26 9:00PM</t>
   </si>
@@ -444,6 +444,9 @@
   </si>
   <si>
     <t>I can't F Nov 29, T Dec 4, H Dec 5, my school ends on Dec 3,</t>
+  </si>
+  <si>
+    <t>except 2h30-6h</t>
   </si>
 </sst>
 </file>
@@ -850,7 +853,7 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8:H8"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -894,7 +897,7 @@
         <v>67</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>121</v>

</xml_diff>

<commit_message>
quick fix for except (in the handling of double ranges in get_practice_range() method)
</commit_message>
<xml_diff>
--- a/test_twice.xlsx
+++ b/test_twice.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/seasy/Documents/Projects/PM-Replacement/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A2261A5-F73D-F749-8217-3A84FFEB9A79}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1A860765-CA00-9E4E-9AD4-AB721B937A57}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17540" xr2:uid="{D0A65B29-C4AD-3F43-ADB3-EAE2E589548A}"/>
   </bookViews>
@@ -446,7 +446,7 @@
     <t>I can't F Nov 29, T Dec 4, H Dec 5, my school ends on Dec 3,</t>
   </si>
   <si>
-    <t>except 2h30-6h</t>
+    <t>free except 3-6</t>
   </si>
 </sst>
 </file>
@@ -853,10 +853,14 @@
   <dimension ref="A1:M8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">

</xml_diff>